<commit_message>
Feature/CRMR-3 - Develop Created the promo report and covered all the code with the unit tests
</commit_message>
<xml_diff>
--- a/reports/nce_promos/templates/xlsx/template.xlsx
+++ b/reports/nce_promos/templates/xlsx/template.xlsx
@@ -1,37 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ensim\nce_promo_reports\reports\nce_promos\templates\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9060F7FA-0433-443F-904F-9721A9A19F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$W$1</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Request Type</t>
+  </si>
+  <si>
+    <t>Request ID</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Request Created At</t>
+  </si>
+  <si>
+    <t>Subscription Created At</t>
+  </si>
+  <si>
+    <t>Subscription ID</t>
+  </si>
+  <si>
+    <t>Subscription Status</t>
+  </si>
+  <si>
+    <t>Subscription External ID</t>
+  </si>
+  <si>
+    <t>Promotion Applied (%)</t>
+  </si>
+  <si>
+    <t>Microsoft Tenant ID</t>
+  </si>
+  <si>
+    <t>Microsoft Domain</t>
+  </si>
+  <si>
+    <t>Microsoft Subscription ID</t>
+  </si>
+  <si>
+    <t>Microsoft Order ID</t>
+  </si>
+  <si>
+    <t>Microsoft Plan ID</t>
+  </si>
+  <si>
+    <t>Item ID</t>
+  </si>
+  <si>
+    <t>Item MPN</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>Item Period</t>
+  </si>
+  <si>
+    <t>Item Quantity</t>
+  </si>
+  <si>
+    <t>Marketplace Name</t>
+  </si>
+  <si>
+    <t>Microsoft Tier1 MPN (if any)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,81 +144,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,19 +457,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="14.88671875" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:W1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>